<commit_message>
Got several of the bullet tests working again.
</commit_message>
<xml_diff>
--- a/Libraries/AnimatTesting/TestErrors.xlsx
+++ b/Libraries/AnimatTesting/TestErrors.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-15" yWindow="795" windowWidth="28800" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>Test_Box</t>
   </si>
@@ -131,73 +126,37 @@
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: X90_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\JointTests\DistanceTest\DataTool_1.txt', Column: 'Block_X', row: 9561, Template Value: '0.8566281', Test Data: '0.8266115'</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\EllipsoidTest\DataTool_1.txt', Column: 'Joint_Y', row: 1920, Template Value: '0.09124797', Test Data: '-0.008826593'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: EnableActive_False_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\BodyPartTests\RigidBodyTests\EnablerTest\BodyData.txt', Column: 'Tension', row: 1006, Template Value: '0', Test Data: '0.3995052'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: FallUp90Deg_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\JointTests\HingeTest\DataTool_1.txt', Column: 'JointVelocity', row: 501, Template Value: '-0.1413822', Test Data: '-1.225233'</t>
-  </si>
-  <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: MotorDownVel1_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\JointTests\HingeTest\DataTool_1.txt', Column: 'JointVelocity', row: 8329, Template Value: '0.0002543708', Test Data: '-0.9883649'</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\MeshTest\DataTool_1.txt', Column: 'Joint_Y', row: 2791, Template Value: '0.003761667', Test Data: '0.1039294'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\BodyPartTests\RigidBodyTests\MuscleTest\BodyData.txt', Column: 'Length', row: 40640, Template Value: '0.4999971', Test Data: '0.4596'</t>
-  </si>
-  <si>
     <t>BUG</t>
   </si>
   <si>
-    <t>not stopping when motor disabled.</t>
-  </si>
-  <si>
     <t>missing files, rerun</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\BodyPartTests\RigidBodyTests\ReceptiveFields\BodyData.txt', Column: 'A1', row: 3215, Template Value: '-0.06986341', Test Data: '-0.05977095'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\BodyPartTests\RigidBodyTests\ReceptiveFields_Kg_M\BodyData.txt', Column: '1', row: 352, Template Value: '0.6908142', Test Data: '0.4797751'</t>
-  </si>
-  <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Could not read the template file. ('F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestData\BodyEditorTests\BodyPartTests\RigidBodyTests\Sphere_Friction_dmg\Uk_0_F_20_M_1_DataTool_1.txt')</t>
   </si>
   <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: Uk_0_02_F_20_M_1_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\Sphere_Friction_KgM\DataTool_1.txt', Column: 'Vx', row: 7766, Template Value: '-0.4402355', Test Data: '0'</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\BodyPartTests\RigidBodyTests\StretchReceptorTest\BodyData.txt', Column: 'Length', row: 40635, Template Value: '0.4999971', Test Data: '0.4596'</t>
-  </si>
-  <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\TerrainTest\DataTool_1.txt', Column: 'Root2_Y', row: 1109, Template Value: '0.2075192', Test Data: '0.1072061'</t>
   </si>
   <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\TorusTest\DataTool_1.txt', Column: 'Joint_Y', row: 2389, Template Value: '0.1174236', Test Data: '0.01739641'</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: L_7m_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\BodyPartTests\RigidBodyTests\UnitScale_Kg_M\BodyData.txt', Column: 'PendulumX', row: 6533, Template Value: '6.085013', Test Data: '6.135036'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\TutorialTests\Examples\Belly Flopper\BodyData.txt', Column: 'BodyX', row: 6840, Template Value: '0.003269146', Test Data: '0.002268609'</t>
-  </si>
-  <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\TutorialTests\SensorySystems\Eating\DataChart.txt', Column: 'Contact', row: 410, Template Value: '3', Test Data: '0'</t>
   </si>
   <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\TutorialTests\SensorySystems\Eating\DataChart.txt', Column: 'Eat', row: 432, Template Value: '0.05390253', Test Data: '0'</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\TutorialTests\BodyParts\Muscle\DataChart.txt', Column: 'A', row: 41250, Template Value: '0.01380181', Test Data: '0.002819488'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\TutorialTests\BodyParts\StretchReceptor\DataChart.txt', Column: 'II', row: 5695, Template Value: '152.2992', Test Data: '151.996'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\TutorialTests\SensorySystems\TouchReceptiveFields\DataChart.txt', Column: 'A4', row: 5004, Template Value: '0.01237395', Test Data: '0'</t>
+    <t>Bullet/Vortex</t>
+  </si>
+  <si>
+    <t>Terrain issue again</t>
   </si>
 </sst>
 </file>
@@ -507,7 +466,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,347 +474,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
       <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
       <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21">
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21">
         <v>2</v>
       </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22">
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22">
         <v>3</v>
       </c>
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
       <c r="C28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>33</v>
       </c>
-      <c r="C29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got the eating tests working again.
</commit_message>
<xml_diff>
--- a/Libraries/AnimatTesting/TestErrors.xlsx
+++ b/Libraries/AnimatTesting/TestErrors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>Test_Box</t>
   </si>
@@ -145,12 +145,6 @@
   </si>
   <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\TorusTest\DataTool_1.txt', Column: 'Joint_Y', row: 2389, Template Value: '0.1174236', Test Data: '0.01739641'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\TutorialTests\SensorySystems\Eating\DataChart.txt', Column: 'Contact', row: 410, Template Value: '3', Test Data: '0'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\TutorialTests\SensorySystems\Eating\DataChart.txt', Column: 'Eat', row: 432, Template Value: '0.05390253', Test Data: '0'</t>
   </si>
   <si>
     <t>Bullet/Vortex</t>
@@ -466,7 +460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +635,7 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,7 +733,7 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>31</v>
@@ -785,19 +779,19 @@
       <c r="A28" t="s">
         <v>22</v>
       </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
       <c r="C28" t="s">
         <v>31</v>
       </c>
-      <c r="D28" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
       <c r="C29" t="s">
         <v>33</v>
-      </c>
-      <c r="D29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed the bullet box friction test.
</commit_message>
<xml_diff>
--- a/Libraries/AnimatTesting/TestErrors.xlsx
+++ b/Libraries/AnimatTesting/TestErrors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
   <si>
     <t>Test_Box</t>
   </si>
@@ -102,30 +102,15 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: Uk_1_F_10_M_0_1_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\BoxFriction_KgM\DataTool_1.txt', Column: 'Px', row: 10662, Template Value: '92.01211', Test Data: '91.98208'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: Uk_1_F_10_M_0_1_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\BoxFriction_dmg\DataTool_1.txt', Column: 'Px', row: 11651, Template Value: '99.36063', Test Data: '99.33062'</t>
-  </si>
-  <si>
     <t>System.Exception: Angular Primary Friction was not converted correctly.</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterConversion_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\BodyPartTests\RigidBodyTests\ContactSensors\BodyData.txt', Column: 'CylinderContact', row: 210, Template Value: '0.009028472', Test Data: '0.05977406'</t>
-  </si>
-  <si>
     <t>Bullet</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: DeleteNeuronsBeforeChartOpen_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\ConversionTests\BodyPartTests\RigidBodyTests\ReceptiveFields\BodyData.txt', Column: 'A4', row: 173, Template Value: '-0.06999882', Test Data: '-0.06890725'</t>
-  </si>
-  <si>
     <t>Vortex</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: X90_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\JointTests\DistanceTest\DataTool_1.txt', Column: 'Block_X', row: 9561, Template Value: '0.8566281', Test Data: '0.8266115'</t>
-  </si>
-  <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: MotorDownVel1_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\JointTests\HingeTest\DataTool_1.txt', Column: 'JointVelocity', row: 8329, Template Value: '0.0002543708', Test Data: '-0.9883649'</t>
   </si>
   <si>
@@ -142,9 +127,6 @@
   </si>
   <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\TerrainTest\DataTool_1.txt', Column: 'Root2_Y', row: 1109, Template Value: '0.2075192', Test Data: '0.1072061'</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\TorusTest\DataTool_1.txt', Column: 'Joint_Y', row: 2389, Template Value: '0.1174236', Test Data: '0.01739641'</t>
   </si>
   <si>
     <t>Bullet/Vortex</t>
@@ -470,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +463,7 @@
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,57 +471,57 @@
         <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
       <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -547,24 +529,21 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
       <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -572,10 +551,10 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -583,10 +562,10 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -594,18 +573,18 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -613,10 +592,10 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -624,10 +603,10 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -635,18 +614,18 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -654,7 +633,7 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,7 +644,7 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -676,7 +655,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -686,35 +665,35 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,7 +704,7 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -733,24 +712,24 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
       <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -761,7 +740,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -772,7 +751,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -783,7 +762,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -791,7 +770,7 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -802,7 +781,7 @@
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -813,7 +792,7 @@
         <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -824,7 +803,7 @@
         <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Got the vortex hinge test working again. 2. Made sure all derived test classes implement the Testclenaup method and call the base class to ensure proper cleanup.
</commit_message>
<xml_diff>
--- a/Libraries/AnimatTesting/TestErrors.xlsx
+++ b/Libraries/AnimatTesting/TestErrors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
   <si>
     <t>Test_Box</t>
   </si>
@@ -102,28 +102,16 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>System.Exception: Angular Primary Friction was not converted correctly.</t>
-  </si>
-  <si>
     <t>Bullet</t>
   </si>
   <si>
     <t>Vortex</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: MotorDownVel1_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\JointTests\HingeTest\DataTool_1.txt', Column: 'JointVelocity', row: 8329, Template Value: '0.0002543708', Test Data: '-0.9883649'</t>
-  </si>
-  <si>
     <t>BUG</t>
   </si>
   <si>
     <t>missing files, rerun</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Could not read the template file. ('F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestData\BodyEditorTests\BodyPartTests\RigidBodyTests\Sphere_Friction_dmg\Uk_0_F_20_M_1_DataTool_1.txt')</t>
-  </si>
-  <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: Uk_0_02_F_20_M_1_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\Sphere_Friction_KgM\DataTool_1.txt', Column: 'Vx', row: 7766, Template Value: '-0.4402355', Test Data: '0'</t>
   </si>
   <si>
     <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\TerrainTest\DataTool_1.txt', Column: 'Root2_Y', row: 1109, Template Value: '0.2075192', Test Data: '0.1072061'</t>
@@ -442,7 +430,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -450,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +459,7 @@
         <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -482,7 +470,7 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -493,7 +481,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -503,10 +491,10 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
       <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -518,7 +506,7 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -529,7 +517,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -540,7 +528,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -551,7 +539,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,7 +550,7 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -573,15 +561,15 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -592,7 +580,7 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,7 +591,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,7 +602,7 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,7 +610,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -633,10 +621,10 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -644,10 +632,10 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -655,48 +643,51 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
-      <c r="E22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -704,24 +695,24 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -729,10 +720,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -740,10 +731,10 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -751,10 +742,10 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -762,18 +753,18 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -781,10 +772,10 @@
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -792,10 +783,10 @@
         <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -803,7 +794,7 @@
         <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Fixed a bug in the generation of the bullet terrain height map. It needed to be using btScalar instead of float. When I did double precision it was all messed up. 2. Got the terrain test for bullet working again with double precision.
</commit_message>
<xml_diff>
--- a/Libraries/AnimatTesting/TestErrors.xlsx
+++ b/Libraries/AnimatTesting/TestErrors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
   <si>
     <t>Test_Box</t>
   </si>
@@ -114,13 +114,7 @@
     <t>missing files, rerun</t>
   </si>
   <si>
-    <t>System.Reflection.TargetInvocationException: Exception has been thrown by the target of an invocation. ---&gt; System.Exception: Data mismatch for test: AfterStruct_ file: 'F:\Projects\AnimatLabSDK\AnimatLabPublicSource\Libraries\AnimatTesting\TestProjects\BodyEditorTests\BodyPartTests\RigidBodyTests\TerrainTest\DataTool_1.txt', Column: 'Root2_Y', row: 1109, Template Value: '0.2075192', Test Data: '0.1072061'</t>
-  </si>
-  <si>
     <t>Bullet/Vortex</t>
-  </si>
-  <si>
-    <t>Terrain issue again</t>
   </si>
 </sst>
 </file>
@@ -430,7 +424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,7 +435,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +596,7 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -703,13 +697,10 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>